<commit_message>
Optimize Excel input experience and add unified builder
- Remove highlightEvery and dateFormat from user-facing config (hard-coded in rendering)
- Remove color column from Tasks sheet (auto-assigned from SEI palette)
- Replace taskIndex with linkedTask dropdown in Milestones sheet
- Add unified build.js script that accepts JSON or XLSX input
- Move real project data to gitignored input/ directory
- Create example beverage machine upgrade project template
- Update Excel template generator with new example project
- Remove CSV template (Excel is primary format)
- Auto-open Excel template after generation
- Update all documentation and README
</commit_message>
<xml_diff>
--- a/templates/gantt_template.xlsx
+++ b/templates/gantt_template.xlsx
@@ -30,14 +30,14 @@
     <comment ref="B1" authorId="0">
       <text>
         <r>
-          <t>Start date in YYYY-MM-DD format (e.g., "2025-12-01")</t>
+          <t>Start date in YYYY-MM-DD format (e.g., "2025-01-06")</t>
         </r>
       </text>
     </comment>
     <comment ref="C1" authorId="0">
       <text>
         <r>
-          <t>End date in YYYY-MM-DD format (e.g., "2026-02-14")</t>
+          <t>End date in YYYY-MM-DD format (e.g., "2025-03-14")</t>
         </r>
       </text>
     </comment>
@@ -45,20 +45,6 @@
       <text>
         <r>
           <t>Show milestones? (true or false)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E1" authorId="0">
-      <text>
-        <r>
-          <t>Highlight every Nth day (number, e.g., 5)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F1" authorId="0">
-      <text>
-        <r>
-          <t>Date format: "short" or "long"</t>
         </r>
       </text>
     </comment>
@@ -174,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="88">
   <si>
     <t>📊 GANTT CHART TEMPLATE - INSTRUCTIONS</t>
   </si>
@@ -184,7 +170,7 @@
   <si>
     <t xml:space="preserve">This template allows you to create a professional Gantt chart by filling in the data sheets below. Each sheet has a specific purpose:
 • PROJECT: Set the overall timeline and chart settings
-• TASKS: Define your project tasks with dates, colors, and subtasks
+• TASKS: Define your project tasks with dates and subtasks (colors are assigned automatically)
 • MILESTONES: Mark important project milestones
 • PAUSE_PERIODS: Define any breaks or holidays (optional)</t>
   </si>
@@ -246,7 +232,7 @@
     <t>Pause periods, neutral elements</t>
   </si>
   <si>
-    <t>💡 TIP: Copy the hex codes above (including the #) into the "color" column in the Tasks sheet. You can use any of these colors or your own custom hex colors.</t>
+    <t>💡 TIP: Colors shown above are from the SEI palette. Task colors are automatically assigned from this palette when you import the data - no manual selection needed!</t>
   </si>
   <si>
     <t>📅 PROJECT SHEET</t>
@@ -254,21 +240,19 @@
   <si>
     <t xml:space="preserve">Fill in ONE row with your project details:
 • title: The chart title (e.g., "PROJECT TIMELINE")
-• timelineStart: Start date in YYYY-MM-DD format (e.g., "2025-12-01")
-• timelineEnd: End date in YYYY-MM-DD format (e.g., "2026-02-14")
-• showMilestones: true or false (default: true)
-• highlightEvery: Number of days between highlights (default: 5)
-• dateFormat: "short" or "long" (default: "short")</t>
+• timelineStart: Start date in YYYY-MM-DD format (e.g., "2025-01-06")
+• timelineEnd: End date in YYYY-MM-DD format (e.g., "2025-03-14")
+• showMilestones: true or false (default: true)</t>
   </si>
   <si>
     <t>✅ TASKS SHEET</t>
   </si>
   <si>
     <t xml:space="preserve">Add one row per task. Each task needs:
-• name: Task name (e.g., "Planning &amp; Preparation")
-• start: Start date in YYYY-MM-DD format (e.g., "2025-12-02")
-• end: End date in YYYY-MM-DD format (e.g., "2025-12-14")
-• hours: Estimated hours (number, e.g., 20)
+• name: Task name (e.g., "Planning &amp; Vendor Selection")
+• start: Start date in YYYY-MM-DD format (e.g., "2025-01-06")
+• end: End date in YYYY-MM-DD format (e.g., "2025-01-24")
+• hours: Estimated hours (number, e.g., 30)
 • subtask1 through subtask10: Optional subtasks (up to 10 per task)
 💡 TIP: Colors are automatically assigned! Each task gets a unique color from the SEI palette, and no two adjacent tasks will have the same color.
 💡 TIP: Leave subtask columns empty if you have fewer than 10 subtasks.</t>
@@ -279,7 +263,7 @@
   <si>
     <t xml:space="preserve">Add one row per milestone:
 • name: Milestone name (use \n for line breaks, e.g., "Project\nKickoff")
-• date: Milestone date in YYYY-MM-DD format (e.g., "2025-12-02")
+• date: Milestone date in YYYY-MM-DD format (e.g., "2025-01-06")
 • linkedTask: Select the associated task from the dropdown list (or leave blank)
 💡 TIP: The linkedTask column has a dropdown menu showing all tasks from the Tasks sheet. Simply click the cell and select from the list!
 💡 TIP: You can leave linkedTask blank if the milestone is not associated with a specific task.</t>
@@ -289,8 +273,8 @@
   </si>
   <si>
     <t xml:space="preserve">Add one row per pause/break period:
-• start: Pause start date in YYYY-MM-DD format (e.g., "2025-12-23")
-• end: Pause end date in YYYY-MM-DD format (e.g., "2026-01-04")
+• start: Pause start date in YYYY-MM-DD format (e.g., "2025-02-15")
+• end: Pause end date in YYYY-MM-DD format (e.g., "2025-02-17")
 💡 TIP: Leave this sheet empty if you have no pause periods. Tasks that span a pause will automatically show a break effect.</t>
   </si>
   <si>
@@ -300,8 +284,8 @@
     <t xml:space="preserve">• Dates MUST be in YYYY-MM-DD format (e.g., "2025-12-01", not "12/1/2025")
 • Task start dates must be before end dates
 • All task dates must fall within the timeline range
-• Colors are assigned automatically - no need to set them manually
-• Milestone linking is automatic - the formula finds the matching task
+• Task colors are automatically assigned from the SEI palette - no manual selection needed
+• Milestone linking uses a dropdown - select the associated task from the list
 • Use \n in milestone names for line breaks (not actual line breaks)</t>
   </si>
   <si>
@@ -330,22 +314,13 @@
     <t>showMilestones</t>
   </si>
   <si>
-    <t>highlightEvery</t>
-  </si>
-  <si>
-    <t>dateFormat</t>
-  </si>
-  <si>
     <t>PROJECT TIMELINE</t>
   </si>
   <si>
-    <t>2025-12-01</t>
-  </si>
-  <si>
-    <t>2026-02-14</t>
-  </si>
-  <si>
-    <t>short</t>
+    <t>2025-01-06</t>
+  </si>
+  <si>
+    <t>2025-03-14</t>
   </si>
   <si>
     <t>name</t>
@@ -390,58 +365,76 @@
     <t>subtask10</t>
   </si>
   <si>
-    <t>Planning &amp; Preparation</t>
-  </si>
-  <si>
-    <t>2025-12-02</t>
-  </si>
-  <si>
-    <t>2025-12-14</t>
-  </si>
-  <si>
-    <t>Define scope: URLs/Domains to audit; discovery and interviews</t>
-  </si>
-  <si>
-    <t>Determine test personas/scenarios</t>
-  </si>
-  <si>
-    <t>Baseline environment setup, any special access required</t>
+    <t>Planning &amp; Vendor Selection</t>
+  </si>
+  <si>
+    <t>2025-01-24</t>
+  </si>
+  <si>
+    <t>Research beverage machine vendors and models</t>
+  </si>
+  <si>
+    <t>Compare features, pricing, and maintenance requirements</t>
+  </si>
+  <si>
+    <t>Schedule vendor demos and site visits</t>
+  </si>
+  <si>
+    <t>Evaluate compatibility with existing POS systems</t>
+  </si>
+  <si>
+    <t>Select vendor and negotiate contract terms</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>Initial Site Scans – Tracking System</t>
-  </si>
-  <si>
-    <t>2025-12-15</t>
-  </si>
-  <si>
-    <t>2026-01-11</t>
-  </si>
-  <si>
-    <t>Scan site and mobile app</t>
-  </si>
-  <si>
-    <t>Capture all tracking artifacts (cookies, storage, third party scripts, beacons/pixels)</t>
-  </si>
-  <si>
-    <t>Log and classify by purpose/category</t>
-  </si>
-  <si>
-    <t>Consent Mechanism Testing</t>
-  </si>
-  <si>
-    <t>2026-01-12</t>
-  </si>
-  <si>
-    <t>2026-01-25</t>
-  </si>
-  <si>
-    <t>Opt out of all cookies, verify deactivation across user journeys</t>
-  </si>
-  <si>
-    <t>Audit site/app data flow compliance and messaging for GPC/DNSS signals</t>
+    <t>Site Preparation &amp; Installation</t>
+  </si>
+  <si>
+    <t>2025-01-27</t>
+  </si>
+  <si>
+    <t>2025-02-21</t>
+  </si>
+  <si>
+    <t>Coordinate with facilities team for electrical and plumbing requirements</t>
+  </si>
+  <si>
+    <t>Schedule installation during off-peak hours</t>
+  </si>
+  <si>
+    <t>Remove old beverage machine and dispose of equipment</t>
+  </si>
+  <si>
+    <t>Install new machine and connect to utilities</t>
+  </si>
+  <si>
+    <t>Test all connections and basic functionality</t>
+  </si>
+  <si>
+    <t>System Integration &amp; Testing</t>
+  </si>
+  <si>
+    <t>2025-02-24</t>
+  </si>
+  <si>
+    <t>2025-03-07</t>
+  </si>
+  <si>
+    <t>Integrate new machine with POS system</t>
+  </si>
+  <si>
+    <t>Configure menu items and pricing</t>
+  </si>
+  <si>
+    <t>Test payment processing and receipt printing</t>
+  </si>
+  <si>
+    <t>Train staff on new machine operation</t>
+  </si>
+  <si>
+    <t>Conduct end-to-end testing with real orders</t>
   </si>
   <si>
     <t>date</t>
@@ -454,24 +447,20 @@
 Kickoff</t>
   </si>
   <si>
-    <t xml:space="preserve">Testing
+    <t xml:space="preserve">Installation
 Complete</t>
   </si>
   <si>
-    <t xml:space="preserve">Deliver
-Final Report</t>
-  </si>
-  <si>
-    <t>2026-02-09</t>
-  </si>
-  <si>
-    <t>Final Report and Recommendations</t>
-  </si>
-  <si>
-    <t>2025-12-23</t>
-  </si>
-  <si>
-    <t>2026-01-04</t>
+    <t>Go Live</t>
+  </si>
+  <si>
+    <t>Staff Training &amp; Documentation</t>
+  </si>
+  <si>
+    <t>2025-02-15</t>
+  </si>
+  <si>
+    <t>2025-02-17</t>
   </si>
 </sst>
 </file>
@@ -1228,7 +1217,7 @@
       <c r="E16"/>
       <c r="F16"/>
     </row>
-    <row r="17" ht="140" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" ht="120" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>24</v>
       </c>
@@ -1372,7 +1361,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1382,11 +1371,10 @@
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="2" max="4" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="25" customHeight="1" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" ht="25" customHeight="1" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>35</v>
       </c>
@@ -1399,31 +1387,19 @@
       <c r="D1" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="16" t="s">
+    </row>
+    <row r="2" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="B2" s="17" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="C2" s="17" t="s">
         <v>41</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>43</v>
       </c>
       <c r="D2" s="17" t="b">
         <v>1</v>
-      </c>
-      <c r="E2" s="17">
-        <v>5</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1452,134 +1428,134 @@
   <sheetData>
     <row r="1" ht="30" customHeight="1" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="F1" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="G1" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="H1" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="I1" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="J1" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="K1" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="L1" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="M1" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="N1" s="18" t="s">
         <v>55</v>
-      </c>
-      <c r="L1" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="M1" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="N1" s="18" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="19">
+        <v>30</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="G2" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="H2" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="19">
-        <v>20</v>
-      </c>
-      <c r="E2" s="19" t="s">
+      <c r="I2" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="J2" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="G2" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="J2" s="19" t="s">
-        <v>65</v>
-      </c>
       <c r="K2" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L2" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M2" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N2" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="D3" s="19">
+        <v>40</v>
+      </c>
+      <c r="E3" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="F3" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="19">
-        <v>20</v>
-      </c>
-      <c r="E3" s="19" t="s">
+      <c r="G3" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="H3" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="I3" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="H3" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="I3" s="19" t="s">
-        <v>65</v>
-      </c>
       <c r="J3" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K3" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L3" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M3" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N3" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -1593,7 +1569,7 @@
         <v>74</v>
       </c>
       <c r="D4" s="19">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E4" s="19" t="s">
         <v>75</v>
@@ -1602,28 +1578,28 @@
         <v>76</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="H4" s="19" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="I4" s="19" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="J4" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K4" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L4" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M4" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N4" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1651,46 +1627,46 @@
   <sheetData>
     <row r="1" ht="25" customHeight="1" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="3:3" x14ac:dyDescent="0.25"/>
@@ -1820,18 +1796,18 @@
   <sheetData>
     <row r="1" ht="25" customHeight="1" spans="1:2" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Instructions sheet to Excel template and comprehensive Excel guide
- Add Instructions sheet as first sheet in Excel template
- Include quick start guide, sheet reference, and tips
- Create comprehensive Excel template documentation (EXCEL_TEMPLATE_GUIDE.md)
- Document palette system (template vs preset override)
- Add troubleshooting section and workflow examples
</commit_message>
<xml_diff>
--- a/templates/gantt_template.xlsx
+++ b/templates/gantt_template.xlsx
@@ -4,18 +4,151 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Palette" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="Project" state="visible" r:id="rId5"/>
-    <sheet sheetId="3" name="Tasks" state="visible" r:id="rId6"/>
-    <sheet sheetId="4" name="Milestones" state="visible" r:id="rId7"/>
-    <sheet sheetId="5" name="PausePeriods" state="visible" r:id="rId8"/>
+    <sheet sheetId="1" name="Instructions" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Palette" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="Project" state="visible" r:id="rId6"/>
+    <sheet sheetId="4" name="Tasks" state="visible" r:id="rId7"/>
+    <sheet sheetId="5" name="Milestones" state="visible" r:id="rId8"/>
+    <sheet sheetId="6" name="PausePeriods" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="102">
+  <si>
+    <t>GanttGen Excel Template - Instructions</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>QUICK START</t>
+  </si>
+  <si>
+    <t>1. Fill in the Project sheet with your timeline dates</t>
+  </si>
+  <si>
+    <t>2. Add your tasks in the Tasks sheet</t>
+  </si>
+  <si>
+    <t>3. Add milestones in the Milestones sheet (optional)</t>
+  </si>
+  <si>
+    <t>4. Add pause periods if needed (optional)</t>
+  </si>
+  <si>
+    <t>5. Run: node scripts/build.js --input your_file.xlsx --palette alternating_b</t>
+  </si>
+  <si>
+    <t>SHEET GUIDE</t>
+  </si>
+  <si>
+    <t>Sheet Name</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Palette</t>
+  </si>
+  <si>
+    <t>Color definitions</t>
+  </si>
+  <si>
+    <t>Optional*</t>
+  </si>
+  <si>
+    <t>*Palette preset flag overrides this</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Timeline &amp; settings</t>
+  </si>
+  <si>
+    <t>Set start/end dates and title</t>
+  </si>
+  <si>
+    <t>Tasks</t>
+  </si>
+  <si>
+    <t>Task definitions</t>
+  </si>
+  <si>
+    <t>Add tasks with dates, hours, subtasks</t>
+  </si>
+  <si>
+    <t>Milestones</t>
+  </si>
+  <si>
+    <t>Key milestones</t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <t>Link to tasks via dropdown</t>
+  </si>
+  <si>
+    <t>PausePeriods</t>
+  </si>
+  <si>
+    <t>Break periods</t>
+  </si>
+  <si>
+    <t>Holidays, reviews, etc.</t>
+  </si>
+  <si>
+    <t>COLOR PALETTES</t>
+  </si>
+  <si>
+    <t>Use --palette flag to override template colors:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  • reds, reds_b - Red gradients</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  • purples_a, purples_b, purples_c - Purple gradients</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  • alternating, alternating_b - Red/purple mix (recommended)</t>
+  </si>
+  <si>
+    <t>DATE FORMAT</t>
+  </si>
+  <si>
+    <t>All dates must be in YYYY-MM-DD format (e.g., 2025-01-15)</t>
+  </si>
+  <si>
+    <t>TIPS</t>
+  </si>
+  <si>
+    <t>• Use colorIndex in Tasks sheet to reference Palette colors (0-based)</t>
+  </si>
+  <si>
+    <t>• Milestones link to tasks via dropdown menu</t>
+  </si>
+  <si>
+    <t>• Tasks spanning pause periods show diagonal stripe breaks</t>
+  </si>
+  <si>
+    <t>• Leave empty cells if you have fewer than 10 subtasks</t>
+  </si>
+  <si>
+    <t>DOCUMENTATION</t>
+  </si>
+  <si>
+    <t>See docs/EXCEL_TEMPLATE_GUIDE.md for detailed instructions</t>
+  </si>
   <si>
     <t>color</t>
   </si>
@@ -120,9 +253,6 @@
   </si>
   <si>
     <t>Initial assessment</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>Phase 2: Planning</t>
@@ -198,7 +328,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -209,17 +339,49 @@
     <font>
       <b/>
       <color rgb="FFFFFFFF"/>
+      <sz val="16"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="FFFFFFFF"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <sz val="11"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="FFFFFFFF"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
     </font>
     <font>
       <color rgb="FF2C3E50"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2C3E50"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3498DB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF27AE60"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -258,17 +420,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF3498DB"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF0F0F0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF27AE60"/>
       </patternFill>
     </fill>
     <fill>
@@ -359,33 +511,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -725,6 +887,500 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="50" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="40" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="35" customHeight="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" ht="25" customHeight="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" ht="25" customHeight="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" ht="25" customHeight="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" ht="25" customHeight="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" ht="25" customHeight="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" ht="25" customHeight="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" ht="25" customHeight="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A35:D35"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -737,39 +1393,39 @@
     <col min="1" max="1" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="25" customHeight="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>6</v>
+    <row r="1" ht="25" customHeight="1" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -778,7 +1434,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -793,31 +1449,31 @@
     <col min="2" max="4" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="25" customHeight="1" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="9" t="b">
+    <row r="1" ht="25" customHeight="1" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="15" t="b">
         <v>1</v>
       </c>
     </row>
@@ -827,7 +1483,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P5"/>
   <sheetViews>
@@ -845,253 +1501,253 @@
     <col min="15" max="16" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="30" customHeight="1" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="10" t="s">
+    <row r="1" ht="30" customHeight="1" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="N1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="O1" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="17">
+        <v>40</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="18">
+        <v>30</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="P3" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="19">
+        <v>60</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="P4" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="20">
         <v>20</v>
       </c>
-      <c r="H1" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="O1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="11">
-        <v>40</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="O2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="P2" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="12">
-        <v>30</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="N3" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="O3" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="P3" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="13">
-        <v>60</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="L4" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M4" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="N4" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="O4" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="P4" s="13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" s="14">
-        <v>20</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="J5" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="L5" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="M5" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="N5" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="O5" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="P5" s="14">
+      <c r="E5" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="M5" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="N5" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="O5" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="P5" s="20">
         <v>3</v>
       </c>
     </row>
@@ -1101,7 +1757,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C100"/>
   <sheetViews>
@@ -1117,48 +1773,48 @@
     <col min="3" max="3" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="25" customHeight="1" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+    <row r="1" ht="25" customHeight="1" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>48</v>
+      <c r="B1" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="3:3" x14ac:dyDescent="0.25"/>
@@ -1271,7 +1927,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
@@ -1285,12 +1941,12 @@
     <col min="1" max="2" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="25" customHeight="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
+    <row r="1" ht="25" customHeight="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>